<commit_message>
Error en apoyo corregido
</commit_message>
<xml_diff>
--- a/codigo/2D/ejemplo_T3/python/malla_refinada_v2.xlsx
+++ b/codigo/2D/ejemplo_T3/python/malla_refinada_v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="xnod" sheetId="1" state="visible" r:id="rId2"/>
@@ -465,6 +465,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.68367346938776"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -19175,6 +19178,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.68367346938776"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -63761,13 +63767,15 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.68367346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.68367346938776"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -63808,7 +63816,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0</v>
@@ -63838,6 +63846,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.68367346938776"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -64164,11 +64175,14 @@
   </sheetPr>
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.68367346938776"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
@@ -64665,6 +64679,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.68367346938776"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>